<commit_message>
komplet radii Yamaha, tuz przed logika energii
</commit_message>
<xml_diff>
--- a/Kurasik/doc/AV/Yamaha WXAD-10 - lista.xlsx
+++ b/Kurasik/doc/AV/Yamaha WXAD-10 - lista.xlsx
@@ -218,7 +218,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +228,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,6 +261,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,7 +573,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E22" sqref="E22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,36 +609,38 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="6"/>
+      <c r="D3" s="3">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="6"/>
+      <c r="D4" s="3">
         <v>22</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>19</v>
       </c>
     </row>

</xml_diff>